<commit_message>
Removing RC and CA descriptions now included in WPTT data repo
</commit_message>
<xml_diff>
--- a/inputs/FIELDS_STD_SF_DATA.xlsx
+++ b/inputs/FIELDS_STD_SF_DATA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\Dissemination\iotc-metadata-fl\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data-processing\iotc-sf-data-processing\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F265559-4971-48B9-85D1-A4B55602D292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE4C5B3-5EBC-470D-AC50-73B66EBE2DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="669" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="669" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WIDE FORMAT FIELDS - LEGACY" sheetId="16" r:id="rId1"/>
@@ -1060,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6956E8BC-8F37-4832-BD47-15375277A237}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73AFB39F-014D-4912-99D6-2E656A5A2611}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>